<commit_message>
mail function is almost ready
</commit_message>
<xml_diff>
--- a/kayitlar.xlsx
+++ b/kayitlar.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B58"/>
+  <dimension ref="A1:B371"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,7 +444,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[8 61.69 '23.38' 1508.5 10]</t>
+          <t>[10 65.3 '30.61' 3136.0 30]</t>
         </is>
       </c>
     </row>
@@ -454,7 +454,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[8 61.69 '23.38' 1508.5 10]</t>
+          <t>[10 65.3 '30.61' 3136.0 30]</t>
         </is>
       </c>
     </row>
@@ -464,7 +464,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[8 61.69 '23.38' 1508.5 10]</t>
+          <t>[7 65.3 '30.61' 3136.0 30]</t>
         </is>
       </c>
     </row>
@@ -474,7 +474,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[8 61.69 '23.38' 1508.5 10]</t>
+          <t>[7 65.3 '30.61' 3136.0 30]</t>
         </is>
       </c>
     </row>
@@ -484,7 +484,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>[8 61.69 '23.38' 1508.5 10]</t>
+          <t>[7 65.3 '30.61' 3136.0 30]</t>
         </is>
       </c>
     </row>
@@ -494,7 +494,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>[9 61.69 '23.38' 1508.5 10]</t>
+          <t>[7 65.3 '30.61' 3136.0 30]</t>
         </is>
       </c>
     </row>
@@ -504,7 +504,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[9 61.69 '23.38' 1508.5 10]</t>
+          <t>[7 65.3 '30.61' 3136.0 30]</t>
         </is>
       </c>
     </row>
@@ -514,7 +514,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[9 61.69 '23.38' 1508.5 10]</t>
+          <t>[11 65.3 '30.61' 3136.0 30]</t>
         </is>
       </c>
     </row>
@@ -524,7 +524,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[9 61.69 '23.38' 1508.5 10]</t>
+          <t>[11 65.3 '30.61' 3136.0 30]</t>
         </is>
       </c>
     </row>
@@ -534,7 +534,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>[9 61.69 '23.38' 1508.5 10]</t>
+          <t>[11 65.3 '30.61' 3136.0 30]</t>
         </is>
       </c>
     </row>
@@ -544,7 +544,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[9 61.69 '23.38' 1508.5 10]</t>
+          <t>[11 65.3 '30.61' 3136.0 30]</t>
         </is>
       </c>
     </row>
@@ -554,7 +554,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>[9 61.69 '23.38' 1508.5 10]</t>
+          <t>[11 65.3 '30.61' 3136.0 30]</t>
         </is>
       </c>
     </row>
@@ -564,7 +564,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>[9 61.69 '23.38' 1508.5 10]</t>
+          <t>[11 65.3 '30.61' 3136.0 30]</t>
         </is>
       </c>
     </row>
@@ -574,7 +574,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>[9 61.69 '23.38' 1508.5 10]</t>
+          <t>[11 65.3 '30.61' 3136.0 30]</t>
         </is>
       </c>
     </row>
@@ -584,7 +584,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>[9 61.69 '23.38' 1508.5 10]</t>
+          <t>[11 65.3 '30.61' 3136.0 30]</t>
         </is>
       </c>
     </row>
@@ -594,7 +594,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>[9 61.69 '23.38' 1508.5 10]</t>
+          <t>[12 65.3 '30.61' 3136.0 30]</t>
         </is>
       </c>
     </row>
@@ -604,7 +604,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>[9 61.69 '23.38' 1508.5 10]</t>
+          <t>[12 65.3 '30.61' 3136.0 30]</t>
         </is>
       </c>
     </row>
@@ -614,7 +614,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>[9 61.69 '23.38' 1508.5 10]</t>
+          <t>[12 65.3 '30.61' 3136.0 30]</t>
         </is>
       </c>
     </row>
@@ -624,7 +624,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>[9 61.69 '23.38' 1508.5 10]</t>
+          <t>[12 65.3 '30.61' 3136.0 30]</t>
         </is>
       </c>
     </row>
@@ -634,7 +634,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>[9 61.69 '23.38' 1508.5 10]</t>
+          <t>[12 65.3 '30.61' 3136.0 30]</t>
         </is>
       </c>
     </row>
@@ -644,7 +644,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>[9 61.69 '23.38' 1508.5 10]</t>
+          <t>[12 65.3 '30.61' 3136.0 30]</t>
         </is>
       </c>
     </row>
@@ -654,7 +654,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>[12 87.61 '75.23' 6440.0 50]</t>
+          <t>[12 65.3 '30.61' 3136.0 30]</t>
         </is>
       </c>
     </row>
@@ -664,7 +664,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>[17 87.61 '75.23' 6440.0 50]</t>
+          <t>[21 79.78 '59.55' 6440.0 50]</t>
         </is>
       </c>
     </row>
@@ -674,7 +674,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>[16 87.61 '75.23' 6440.0 50]</t>
+          <t>[21 79.78 '59.55' 6440.0 50]</t>
         </is>
       </c>
     </row>
@@ -684,7 +684,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>[16 87.61 '75.23' 6440.0 50]</t>
+          <t>[21 79.78 '59.55' 6440.0 50]</t>
         </is>
       </c>
     </row>
@@ -694,7 +694,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>[16 87.61 '75.23' 6440.0 50]</t>
+          <t>[21 79.78 '59.55' 6440.0 50]</t>
         </is>
       </c>
     </row>
@@ -704,7 +704,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>[16 87.61 '75.23' 6440.0 50]</t>
+          <t>[21 79.78 '59.55' 6440.0 50]</t>
         </is>
       </c>
     </row>
@@ -714,7 +714,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>[16 81.0 '62.00' 6440.0 50]</t>
+          <t>[21 79.78 '59.55' 6440.0 50]</t>
         </is>
       </c>
     </row>
@@ -724,7 +724,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>[16 87.61 '75.23' 6440.0 50]</t>
+          <t>[21 79.78 '59.55' 6440.0 50]</t>
         </is>
       </c>
     </row>
@@ -734,7 +734,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>[16 81.0 '62.00' 6440.0 50]</t>
+          <t>[21 79.78 '59.55' 6440.0 50]</t>
         </is>
       </c>
     </row>
@@ -744,7 +744,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>[16 87.61 '75.23' 6440.0 50]</t>
+          <t>[24 79.78 '59.55' 6440.0 50]</t>
         </is>
       </c>
     </row>
@@ -754,7 +754,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>[16 81.0 '62.00' 6440.0 50]</t>
+          <t>[24 79.78 '59.55' 6440.0 50]</t>
         </is>
       </c>
     </row>
@@ -764,7 +764,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>[16 87.61 '75.23' 6440.0 50]</t>
+          <t>[24 79.78 '59.55' 6440.0 50]</t>
         </is>
       </c>
     </row>
@@ -774,7 +774,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>[16 81.0 '62.00' 6440.0 50]</t>
+          <t>[24 79.78 '59.55' 6440.0 50]</t>
         </is>
       </c>
     </row>
@@ -784,7 +784,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>[12 87.61 '75.23' 6440.0 50]</t>
+          <t>[24 79.78 '59.55' 6440.0 50]</t>
         </is>
       </c>
     </row>
@@ -794,7 +794,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>[12 87.61 '75.23' 6440.0 50]</t>
+          <t>[24 79.78 '59.55' 6440.0 50]</t>
         </is>
       </c>
     </row>
@@ -804,7 +804,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>[12 87.61 '75.23' 6440.0 50]</t>
+          <t>[31 57.28 '14.55' 1508.5 10]</t>
         </is>
       </c>
     </row>
@@ -814,7 +814,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>[12 87.61 '75.23' 6440.0 50]</t>
+          <t>[31 57.28 '14.55' 1508.5 10]</t>
         </is>
       </c>
     </row>
@@ -824,7 +824,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>[12 87.61 '75.23' 6440.0 50]</t>
+          <t>[31 57.28 '14.55' 1508.5 10]</t>
         </is>
       </c>
     </row>
@@ -834,7 +834,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>[12 87.61 '75.23' 6440.0 50]</t>
+          <t>[31 57.28 '14.55' 1508.5 10]</t>
         </is>
       </c>
     </row>
@@ -844,7 +844,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>[12 87.61 '75.23' 6440.0 50]</t>
+          <t>[31 57.28 '14.55' 1508.5 10]</t>
         </is>
       </c>
     </row>
@@ -854,7 +854,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>[12 87.61 '75.23' 6440.0 50]</t>
+          <t>[31 57.28 '14.55' 1508.5 10]</t>
         </is>
       </c>
     </row>
@@ -864,7 +864,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>[12 87.61 '75.23' 6440.0 50]</t>
+          <t>[31 57.28 '14.55' 1508.5 10]</t>
         </is>
       </c>
     </row>
@@ -874,7 +874,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>[12 87.61 '75.23' 6440.0 50]</t>
+          <t>[31 57.28 '14.55' 1508.5 10]</t>
         </is>
       </c>
     </row>
@@ -884,7 +884,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>[12 87.61 '75.23' 6440.0 50]</t>
+          <t>[31 57.28 '14.55' 1508.5 10]</t>
         </is>
       </c>
     </row>
@@ -894,7 +894,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>[12 87.61 '75.23' 6440.0 50]</t>
+          <t>[32 57.28 '14.55' 1508.5 10]</t>
         </is>
       </c>
     </row>
@@ -904,7 +904,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>[12 87.61 '75.23' 6440.0 50]</t>
+          <t>[32 57.28 '14.55' 1508.5 10]</t>
         </is>
       </c>
     </row>
@@ -914,7 +914,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>[12 87.61 '75.23' 6440.0 50]</t>
+          <t>[32 57.28 '14.55' 1508.5 10]</t>
         </is>
       </c>
     </row>
@@ -924,7 +924,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>[12 87.61 '75.23' 6440.0 50]</t>
+          <t>[32 57.28 '14.55' 1508.5 10]</t>
         </is>
       </c>
     </row>
@@ -934,7 +934,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>[12 87.61 '75.23' 6440.0 50]</t>
+          <t>[32 57.28 '14.55' 1508.5 10]</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>[12 87.61 '75.23' 6440.0 50]</t>
+          <t>[32 57.28 '14.55' 1508.5 10]</t>
         </is>
       </c>
     </row>
@@ -954,7 +954,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>[11 76.42 '52.83' 6440.0 50]</t>
+          <t>[32 57.28 '14.55' 1508.5 10]</t>
         </is>
       </c>
     </row>
@@ -964,7 +964,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>[11 76.42 '52.83' 6440.0 50]</t>
+          <t>[32 57.28 '14.55' 1508.5 10]</t>
         </is>
       </c>
     </row>
@@ -974,7 +974,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>[11 76.42 '52.83' 6440.0 50]</t>
+          <t>[32 57.28 '14.55' 1508.5 10]</t>
         </is>
       </c>
     </row>
@@ -984,7 +984,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>[11 76.42 '52.83' 6440.0 50]</t>
+          <t>[32 57.28 '14.55' 1508.5 10]</t>
         </is>
       </c>
     </row>
@@ -994,7 +994,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>[11 76.42 '52.83' 6440.0 50]</t>
+          <t>[32 57.28 '14.55' 1508.5 10]</t>
         </is>
       </c>
     </row>
@@ -1004,7 +1004,3137 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>[11 76.42 '52.83' 6440.0 50]</t>
+          <t>[32 57.28 '14.55' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>[32 57.28 '14.55' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>[32 57.28 '14.55' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>[32 57.28 '14.55' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>[32 57.28 '14.55' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>[32 57.28 '14.55' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>[32 57.28 '14.55' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>[32 57.28 '14.55' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>[32 57.28 '14.55' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>[35 57.28 '14.55' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>[35 57.28 '14.55' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>[35 57.28 '14.55' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>[35 57.28 '14.55' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>[35 57.28 '14.55' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>[35 57.28 '14.55' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>[35 57.28 '14.55' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>[35 57.28 '14.55' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>[35 57.28 '14.55' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>[35 57.28 '14.55' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>[33 57.28 '14.55' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>[33 57.28 '14.55' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>[33 57.28 '14.55' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>[33 57.28 '14.55' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>[33 57.28 '14.55' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>[33 57.28 '14.55' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>[33 57.28 '14.55' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>[40 57.28 '14.55' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>[39 57.28 '14.55' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>[39 58.97 '17.94' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>[39 57.28 '14.55' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>[39 58.97 '17.94' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>[39 58.97 '17.94' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>[38 58.97 '17.94' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>[38 58.97 '17.94' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>[38 58.97 '17.94' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>[38 58.97 '17.94' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>[38 58.97 '17.94' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>[38 58.97 '17.94' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>[41 58.97 '17.94' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>[41 58.97 '17.94' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>[41 58.97 '17.94' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>[41 65.3 '30.61' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>[41 58.97 '17.94' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>[41 65.3 '30.61' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>[41 58.97 '17.94' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>[41 65.3 '30.61' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>102</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>[41 58.97 '17.94' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>103</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>[41 65.3 '30.61' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>[41 58.97 '17.94' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>[41 65.3 '30.61' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>106</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>[41 65.3 '30.61' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>[41 65.3 '30.61' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>[41 65.3 '30.61' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="n">
+        <v>109</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>[41 65.3 '30.61' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>[41 65.3 '30.61' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="n">
+        <v>111</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>[41 65.3 '30.61' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="n">
+        <v>112</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>[41 65.3 '30.61' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="n">
+        <v>113</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>[41 65.3 '30.61' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="n">
+        <v>114</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>[41 65.3 '30.61' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n">
+        <v>115</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>[41 65.3 '30.61' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>[41 65.3 '30.61' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="n">
+        <v>117</v>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>[41 65.3 '30.61' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="n">
+        <v>118</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>[41 65.3 '30.61' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="n">
+        <v>119</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>[41 65.3 '30.61' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>[41 65.3 '30.61' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="n">
+        <v>121</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>[41 65.3 '30.61' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="n">
+        <v>122</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>[41 65.3 '30.61' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="n">
+        <v>123</v>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>[43 58.41 '16.82' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="n">
+        <v>124</v>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>[43 58.41 '16.82' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>[43 58.41 '16.82' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>[43 58.41 '16.82' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="n">
+        <v>127</v>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>[43 58.41 '16.82' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>[43 58.41 '16.82' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>[42 58.41 '16.82' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>[42 58.41 '16.82' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="n">
+        <v>131</v>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>[42 58.41 '16.82' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="n">
+        <v>132</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>[42 58.41 '16.82' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="n">
+        <v>133</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>[42 58.41 '16.82' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>[42 58.41 '16.82' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>[42 58.41 '16.82' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="n">
+        <v>136</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>[42 58.41 '16.82' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="n">
+        <v>137</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>[42 58.41 '16.82' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="n">
+        <v>138</v>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>[42 58.41 '16.82' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>[44 58.41 '16.82' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>[44 58.41 '16.82' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="n">
+        <v>141</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>[44 58.41 '16.82' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="n">
+        <v>142</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>[44 58.41 '16.82' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="n">
+        <v>143</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>[44 58.41 '16.82' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="n">
+        <v>144</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>[42 58.41 '16.82' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>[42 58.41 '16.82' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>[42 58.41 '16.82' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>[42 58.41 '16.82' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="1" t="n">
+        <v>148</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="1" t="n">
+        <v>149</v>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="1" t="n">
+        <v>151</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="1" t="n">
+        <v>152</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="1" t="n">
+        <v>153</v>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="1" t="n">
+        <v>154</v>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="1" t="n">
+        <v>155</v>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="1" t="n">
+        <v>156</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="1" t="n">
+        <v>157</v>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="1" t="n">
+        <v>158</v>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="1" t="n">
+        <v>159</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="1" t="n">
+        <v>160</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="1" t="n">
+        <v>161</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="1" t="n">
+        <v>162</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="1" t="n">
+        <v>163</v>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="1" t="n">
+        <v>164</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="1" t="n">
+        <v>165</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="1" t="n">
+        <v>166</v>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="1" t="n">
+        <v>167</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="1" t="n">
+        <v>168</v>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="1" t="n">
+        <v>169</v>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="1" t="n">
+        <v>170</v>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="1" t="n">
+        <v>171</v>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="1" t="n">
+        <v>172</v>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="1" t="n">
+        <v>173</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="1" t="n">
+        <v>174</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="1" t="n">
+        <v>175</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="1" t="n">
+        <v>176</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="1" t="n">
+        <v>177</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="1" t="n">
+        <v>178</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="1" t="n">
+        <v>179</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="1" t="n">
+        <v>180</v>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="1" t="n">
+        <v>181</v>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="1" t="n">
+        <v>182</v>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="1" t="n">
+        <v>183</v>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="1" t="n">
+        <v>184</v>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="1" t="n">
+        <v>185</v>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="1" t="n">
+        <v>186</v>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>[46 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="1" t="n">
+        <v>187</v>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>[47 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="1" t="n">
+        <v>188</v>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>[47 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="1" t="n">
+        <v>189</v>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>[47 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="1" t="n">
+        <v>190</v>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>[47 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="1" t="n">
+        <v>191</v>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>[47 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="1" t="n">
+        <v>192</v>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>[47 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="1" t="n">
+        <v>193</v>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>[47 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="1" t="n">
+        <v>194</v>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>[47 69.68 '39.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="1" t="n">
+        <v>195</v>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>[49 63.26 '26.53' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="1" t="n">
+        <v>196</v>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>[49 63.26 '26.53' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="1" t="n">
+        <v>197</v>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>[49 63.26 '26.53' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="1" t="n">
+        <v>198</v>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>[49 63.26 '26.53' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="1" t="n">
+        <v>199</v>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>[49 63.26 '26.53' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>[49 63.26 '26.53' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>[49 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="1" t="n">
+        <v>202</v>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>[49 63.26 '26.53' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="1" t="n">
+        <v>203</v>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>[49 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="1" t="n">
+        <v>204</v>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>[49 63.26 '26.53' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" s="1" t="n">
+        <v>205</v>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>[49 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" s="1" t="n">
+        <v>206</v>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>[49 63.26 '26.53' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="1" t="n">
+        <v>207</v>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>[49 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" s="1" t="n">
+        <v>208</v>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>[49 63.26 '26.53' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" s="1" t="n">
+        <v>209</v>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>[49 63.26 '26.53' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="1" t="n">
+        <v>210</v>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>[49 63.26 '26.53' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" s="1" t="n">
+        <v>211</v>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>[49 63.26 '26.53' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" s="1" t="n">
+        <v>212</v>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>[49 63.26 '26.53' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="1" t="n">
+        <v>213</v>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>[52 63.26 '26.53' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="1" t="n">
+        <v>214</v>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>[52 63.26 '26.53' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="1" t="n">
+        <v>215</v>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>[52 63.26 '26.53' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="1" t="n">
+        <v>216</v>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>[52 63.26 '26.53' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="1" t="n">
+        <v>217</v>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>[52 63.26 '26.53' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="1" t="n">
+        <v>218</v>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>[52 63.26 '26.53' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="1" t="n">
+        <v>219</v>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>[52 63.26 '26.53' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="1" t="n">
+        <v>220</v>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>[52 63.26 '26.53' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="1" t="n">
+        <v>221</v>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>[52 63.26 '26.53' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="1" t="n">
+        <v>222</v>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>[52 63.26 '26.53' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="1" t="n">
+        <v>223</v>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>[54 63.26 '26.53' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="1" t="n">
+        <v>224</v>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>[54 63.26 '26.53' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="1" t="n">
+        <v>225</v>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>[54 63.26 '26.53' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="1" t="n">
+        <v>226</v>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>[54 63.26 '26.53' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="1" t="n">
+        <v>227</v>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>[54 63.26 '26.53' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" s="1" t="n">
+        <v>228</v>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>[54 63.26 '26.53' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" s="1" t="n">
+        <v>229</v>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>[56 87.61 '75.23' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" s="1" t="n">
+        <v>230</v>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>[56 87.61 '75.23' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" s="1" t="n">
+        <v>231</v>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>[56 87.61 '75.23' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="1" t="n">
+        <v>232</v>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>[56 87.61 '75.23' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="1" t="n">
+        <v>233</v>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>[56 87.61 '75.23' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" s="1" t="n">
+        <v>234</v>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>[56 87.61 '75.23' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="1" t="n">
+        <v>235</v>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>[56 87.61 '75.23' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" s="1" t="n">
+        <v>236</v>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>[56 87.61 '75.23' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" s="1" t="n">
+        <v>237</v>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>[56 87.61 '75.23' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" s="1" t="n">
+        <v>238</v>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>[56 87.61 '75.23' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" s="1" t="n">
+        <v>239</v>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>[56 87.61 '75.23' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" s="1" t="n">
+        <v>240</v>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>[56 87.61 '75.23' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" s="1" t="n">
+        <v>241</v>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>[56 87.61 '75.23' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" s="1" t="n">
+        <v>242</v>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>[56 87.61 '75.23' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" s="1" t="n">
+        <v>243</v>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>[56 87.61 '75.23' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" s="1" t="n">
+        <v>244</v>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>[56 87.61 '75.23' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" s="1" t="n">
+        <v>245</v>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>[56 87.61 '75.23' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" s="1" t="n">
+        <v>246</v>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>[56 87.61 '75.23' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" s="1" t="n">
+        <v>247</v>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>[56 87.61 '75.23' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" s="1" t="n">
+        <v>248</v>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>[56 87.61 '75.23' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" s="1" t="n">
+        <v>249</v>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>[56 87.61 '75.23' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" s="1" t="n">
+        <v>250</v>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>[56 87.61 '75.23' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" s="1" t="n">
+        <v>251</v>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>[59 87.61 '75.23' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" s="1" t="n">
+        <v>252</v>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>[59 87.61 '75.23' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" s="1" t="n">
+        <v>253</v>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>[59 87.61 '75.23' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" s="1" t="n">
+        <v>254</v>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>[59 87.61 '75.23' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>[59 76.84 '53.69' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" s="1" t="n">
+        <v>256</v>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>[59 76.84 '53.69' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" s="1" t="n">
+        <v>257</v>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>[59 76.84 '53.69' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" s="1" t="n">
+        <v>258</v>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>[59 76.84 '53.69' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" s="1" t="n">
+        <v>259</v>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>[59 76.84 '53.69' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" s="1" t="n">
+        <v>260</v>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>[68 69.21 '38.41' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" s="1" t="n">
+        <v>261</v>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>[68 69.21 '38.41' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" s="1" t="n">
+        <v>262</v>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>[68 69.21 '38.41' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" s="1" t="n">
+        <v>263</v>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>[68 69.21 '38.41' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" s="1" t="n">
+        <v>264</v>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>[68 69.21 '38.41' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" s="1" t="n">
+        <v>265</v>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>[68 69.21 '38.41' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" s="1" t="n">
+        <v>266</v>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>[68 69.21 '38.41' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" s="1" t="n">
+        <v>267</v>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>[68 69.21 '38.41' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" s="1" t="n">
+        <v>268</v>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>[69 69.21 '38.41' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" s="1" t="n">
+        <v>269</v>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>[69 69.21 '38.41' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" s="1" t="n">
+        <v>270</v>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>[69 94.81 '89.62' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" s="1" t="n">
+        <v>271</v>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>[69 69.21 '38.41' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" s="1" t="n">
+        <v>272</v>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>[69 94.81 '89.62' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" s="1" t="n">
+        <v>273</v>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>[69 69.21 '38.41' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" s="1" t="n">
+        <v>274</v>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>[69 94.81 '89.62' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" s="1" t="n">
+        <v>275</v>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>[69 69.21 '38.41' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" s="1" t="n">
+        <v>276</v>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>[69 94.81 '89.62' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" s="1" t="n">
+        <v>277</v>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>[69 69.21 '38.41' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" s="1" t="n">
+        <v>278</v>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>[69 94.81 '89.62' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" s="1" t="n">
+        <v>279</v>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>[69 69.21 '38.41' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" s="1" t="n">
+        <v>280</v>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>[69 94.81 '89.62' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" s="1" t="n">
+        <v>281</v>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>[69 69.21 '38.41' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" s="1" t="n">
+        <v>282</v>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>[69 94.81 '89.62' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" s="1" t="n">
+        <v>283</v>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>[69 69.21 '38.41' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" s="1" t="n">
+        <v>284</v>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>[69 94.81 '89.62' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" s="1" t="n">
+        <v>285</v>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>[69 69.21 '38.41' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" s="1" t="n">
+        <v>286</v>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>[69 94.81 '89.62' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" s="1" t="n">
+        <v>287</v>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>[68 69.21 '38.41' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" s="1" t="n">
+        <v>288</v>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>[68 69.21 '38.41' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" s="1" t="n">
+        <v>289</v>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>[68 69.21 '38.41' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" s="1" t="n">
+        <v>290</v>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>[68 69.21 '38.41' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" s="1" t="n">
+        <v>291</v>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>[68 69.21 '38.41' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" s="1" t="n">
+        <v>292</v>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>[68 69.21 '38.41' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" s="1" t="n">
+        <v>293</v>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>[71 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" s="1" t="n">
+        <v>294</v>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>[71 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" s="1" t="n">
+        <v>295</v>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>[71 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" s="1" t="n">
+        <v>296</v>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>[71 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" s="1" t="n">
+        <v>297</v>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>[71 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" s="1" t="n">
+        <v>298</v>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>[70 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" s="1" t="n">
+        <v>299</v>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>[70 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>[73 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" s="1" t="n">
+        <v>301</v>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>[73 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" s="1" t="n">
+        <v>302</v>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>[73 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" s="1" t="n">
+        <v>303</v>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>[73 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" s="1" t="n">
+        <v>304</v>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>[73 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" s="1" t="n">
+        <v>305</v>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>[73 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" s="1" t="n">
+        <v>306</v>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>[73 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" s="1" t="n">
+        <v>307</v>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>[73 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" s="1" t="n">
+        <v>308</v>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>[73 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" s="1" t="n">
+        <v>309</v>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>[73 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" s="1" t="n">
+        <v>310</v>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>[75 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" s="1" t="n">
+        <v>311</v>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>[75 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" s="1" t="n">
+        <v>312</v>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>[75 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" s="1" t="n">
+        <v>313</v>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>[75 90.56 '81.12' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" s="1" t="n">
+        <v>314</v>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>[75 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" s="1" t="n">
+        <v>315</v>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>[75 90.56 '81.12' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" s="1" t="n">
+        <v>316</v>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>[75 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" s="1" t="n">
+        <v>317</v>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>[75 90.56 '81.12' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" s="1" t="n">
+        <v>318</v>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>[75 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" s="1" t="n">
+        <v>319</v>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>[75 90.56 '81.12' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" s="1" t="n">
+        <v>320</v>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>[75 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" s="1" t="n">
+        <v>321</v>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>[75 90.56 '81.12' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" s="1" t="n">
+        <v>322</v>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>[75 74.68 '49.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" s="1" t="n">
+        <v>323</v>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>[75 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" s="1" t="n">
+        <v>324</v>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>[75 90.56 '81.12' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" s="1" t="n">
+        <v>325</v>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>[75 74.68 '49.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" s="1" t="n">
+        <v>326</v>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>[75 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" s="1" t="n">
+        <v>327</v>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>[75 90.56 '81.12' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" s="1" t="n">
+        <v>328</v>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>[75 74.68 '49.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" s="1" t="n">
+        <v>329</v>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>[75 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" s="1" t="n">
+        <v>330</v>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>[75 90.56 '81.12' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" s="1" t="n">
+        <v>331</v>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>[75 74.68 '49.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" s="1" t="n">
+        <v>332</v>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>[75 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" s="1" t="n">
+        <v>333</v>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>[75 90.56 '81.12' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" s="1" t="n">
+        <v>334</v>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>[75 74.68 '49.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" s="1" t="n">
+        <v>335</v>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>[75 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" s="1" t="n">
+        <v>336</v>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>[75 90.56 '81.12' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" s="1" t="n">
+        <v>337</v>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>[75 74.68 '49.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" s="1" t="n">
+        <v>338</v>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>[75 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" s="1" t="n">
+        <v>339</v>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>[75 90.56 '81.12' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" s="1" t="n">
+        <v>340</v>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>[75 74.68 '49.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" s="1" t="n">
+        <v>341</v>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>[75 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" s="1" t="n">
+        <v>342</v>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>[75 90.56 '81.12' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" s="1" t="n">
+        <v>343</v>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>[75 74.68 '49.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" s="1" t="n">
+        <v>344</v>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>[75 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" s="1" t="n">
+        <v>345</v>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>[75 90.56 '81.12' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" s="1" t="n">
+        <v>346</v>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>[75 74.68 '49.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" s="1" t="n">
+        <v>347</v>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>[75 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" s="1" t="n">
+        <v>348</v>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>[75 90.56 '81.12' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" s="1" t="n">
+        <v>349</v>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>[75 74.68 '49.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" s="1" t="n">
+        <v>350</v>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>[75 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" s="1" t="n">
+        <v>351</v>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>[75 90.56 '81.12' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" s="1" t="n">
+        <v>352</v>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>[75 74.68 '49.36' 3136.0 30]</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" s="1" t="n">
+        <v>353</v>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>[75 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" s="1" t="n">
+        <v>354</v>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>[75 90.56 '81.12' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" s="1" t="n">
+        <v>355</v>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>[75 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" s="1" t="n">
+        <v>356</v>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>[75 90.56 '81.12' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" s="1" t="n">
+        <v>357</v>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>[75 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" s="1" t="n">
+        <v>358</v>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>[75 90.56 '81.12' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" s="1" t="n">
+        <v>359</v>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>[76 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" s="1" t="n">
+        <v>360</v>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>[76 90.56 '81.12' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" s="1" t="n">
+        <v>361</v>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>[76 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" s="1" t="n">
+        <v>362</v>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>[76 90.56 '81.12' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" s="1" t="n">
+        <v>363</v>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>[76 61.69 '23.38' 1508.5 10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" s="1" t="n">
+        <v>364</v>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>[76 90.56 '81.12' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" s="1" t="n">
+        <v>365</v>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>[76 90.56 '81.12' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" s="1" t="n">
+        <v>366</v>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>[76 90.56 '81.12' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" s="1" t="n">
+        <v>367</v>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>[76 90.56 '81.12' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" s="1" t="n">
+        <v>368</v>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>[76 90.56 '81.12' 6440.0 50]</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" s="1" t="n">
+        <v>369</v>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>[76 90.56 '81.12' 6440.0 50]</t>
         </is>
       </c>
     </row>

</xml_diff>